<commit_message>
Daily push for 20200617
</commit_message>
<xml_diff>
--- a/Graphics/20200616/20200616_Kosovo_COVID.xlsx
+++ b/Graphics/20200616/20200616_Kosovo_COVID.xlsx
@@ -590,7 +590,7 @@
         <v>13.05624136759839</v>
       </c>
       <c r="R3" t="n">
-        <v>386.5</v>
+        <v>355.4285714285714</v>
       </c>
       <c r="S3" t="n">
         <v>32.42857142857143</v>
@@ -654,7 +654,7 @@
         <v>9.026729193699175</v>
       </c>
       <c r="R4" t="n">
-        <v>115.124514531675</v>
+        <v>114.1959950030003</v>
       </c>
       <c r="S4" t="n">
         <v>21.84548636962049</v>
@@ -718,7 +718,7 @@
         <v>1.700680272108844</v>
       </c>
       <c r="R5" t="n">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="S5" t="n">
         <v>8</v>
@@ -782,7 +782,7 @@
         <v>6.929283827233816</v>
       </c>
       <c r="R6" t="n">
-        <v>289</v>
+        <v>258.75</v>
       </c>
       <c r="S6" t="n">
         <v>17.5</v>
@@ -846,7 +846,7 @@
         <v>12.41740715424926</v>
       </c>
       <c r="R7" t="n">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="S7" t="n">
         <v>26</v>
@@ -910,7 +910,7 @@
         <v>17.66606265795622</v>
       </c>
       <c r="R8" t="n">
-        <v>448.5</v>
+        <v>417.5</v>
       </c>
       <c r="S8" t="n">
         <v>41.75</v>
@@ -974,7 +974,7 @@
         <v>33.50649350649351</v>
       </c>
       <c r="R9" t="n">
-        <v>652</v>
+        <v>619</v>
       </c>
       <c r="S9" t="n">
         <v>89</v>
@@ -1038,7 +1038,7 @@
         <v>81.48183993638096</v>
       </c>
       <c r="R10" t="n">
-        <v>13253.65384615385</v>
+        <v>13040.72527472528</v>
       </c>
       <c r="S10" t="n">
         <v>477.2252747252747</v>
@@ -1102,7 +1102,7 @@
         <v>0.8265231896042285</v>
       </c>
       <c r="R11" t="n">
-        <v>1.062431806162901</v>
+        <v>1.063948529860846</v>
       </c>
       <c r="S11" t="n">
         <v>1.413594805358087</v>
@@ -1166,7 +1166,7 @@
         <v>0.6293650229936718</v>
       </c>
       <c r="R12" t="n">
-        <v>0.5768314501105598</v>
+        <v>0.5808099381866265</v>
       </c>
       <c r="S12" t="n">
         <v>2.279886783087648</v>
@@ -1230,7 +1230,7 @@
         <v>6.795305822077272</v>
       </c>
       <c r="R13" t="n">
-        <v>89.92857142857143</v>
+        <v>89.26530612244899</v>
       </c>
       <c r="S13" t="n">
         <v>16.63265306122449</v>
@@ -1474,7 +1474,7 @@
         <v>7.720348692365162</v>
       </c>
       <c r="R3" t="n">
-        <v>232.6846846846847</v>
+        <v>217.5315315315315</v>
       </c>
       <c r="S3" t="n">
         <v>13.96846846846847</v>
@@ -1538,7 +1538,7 @@
         <v>7.822494384675468</v>
       </c>
       <c r="R4" t="n">
-        <v>180.5318396487033</v>
+        <v>171.7247702691627</v>
       </c>
       <c r="S4" t="n">
         <v>15.13233733061859</v>
@@ -1666,7 +1666,7 @@
         <v>1.637741710857571</v>
       </c>
       <c r="R6" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S6" t="n">
         <v>2.75</v>
@@ -1730,7 +1730,7 @@
         <v>4.761904761904762</v>
       </c>
       <c r="R7" t="n">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="S7" t="n">
         <v>9</v>
@@ -1794,7 +1794,7 @@
         <v>12.338697984631</v>
       </c>
       <c r="R8" t="n">
-        <v>351.5</v>
+        <v>323</v>
       </c>
       <c r="S8" t="n">
         <v>19.25</v>
@@ -1858,7 +1858,7 @@
         <v>33.50649350649351</v>
       </c>
       <c r="R9" t="n">
-        <v>652</v>
+        <v>619</v>
       </c>
       <c r="S9" t="n">
         <v>89</v>
@@ -1922,7 +1922,7 @@
         <v>61.19141839827923</v>
       </c>
       <c r="R10" t="n">
-        <v>32591.74512694513</v>
+        <v>29489.39672399672</v>
       </c>
       <c r="S10" t="n">
         <v>228.9876330876331</v>
@@ -1986,7 +1986,7 @@
         <v>1.251909007465506</v>
       </c>
       <c r="R11" t="n">
-        <v>0.3475748676607078</v>
+        <v>0.4461600987695634</v>
       </c>
       <c r="S11" t="n">
         <v>1.926408237077894</v>
@@ -2050,7 +2050,7 @@
         <v>1.107244058418083</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.8630875753056308</v>
+        <v>-0.766514674913092</v>
       </c>
       <c r="S12" t="n">
         <v>5.21114402958943</v>
@@ -2114,7 +2114,7 @@
         <v>6.220302675597496</v>
       </c>
       <c r="R13" t="n">
-        <v>146.2033925817711</v>
+        <v>137.2688905121338</v>
       </c>
       <c r="S13" t="n">
         <v>11.10494278061846</v>
@@ -3853,7 +3853,7 @@
         <v>20</v>
       </c>
       <c r="T27" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
@@ -3915,7 +3915,7 @@
         <v>24.7787610619469</v>
       </c>
       <c r="T28" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
@@ -3977,7 +3977,7 @@
         <v>4.761904761904762</v>
       </c>
       <c r="T29" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30">
@@ -4039,7 +4039,7 @@
         <v>23.52941176470588</v>
       </c>
       <c r="T30" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31">
@@ -4101,7 +4101,7 @@
         <v>12.60504201680672</v>
       </c>
       <c r="T31" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32">
@@ -4163,7 +4163,7 @@
         <v>1.886792452830189</v>
       </c>
       <c r="T32" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33">
@@ -4225,7 +4225,7 @@
         <v>6.521739130434782</v>
       </c>
       <c r="T33" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34">
@@ -4287,7 +4287,7 @@
         <v>6.666666666666667</v>
       </c>
       <c r="T34" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35">
@@ -4349,7 +4349,7 @@
         <v>17.39130434782609</v>
       </c>
       <c r="T35" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36">
@@ -4411,7 +4411,7 @@
         <v>5.172413793103448</v>
       </c>
       <c r="T36" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37">
@@ -4473,7 +4473,7 @@
         <v>11.50442477876106</v>
       </c>
       <c r="T37" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38">
@@ -4535,7 +4535,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="T38" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39">
@@ -4597,7 +4597,7 @@
         <v>3.703703703703703</v>
       </c>
       <c r="T39" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40">
@@ -4659,7 +4659,7 @@
         <v>3.90625</v>
       </c>
       <c r="T40" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41">
@@ -4721,7 +4721,7 @@
         <v>5.376344086021505</v>
       </c>
       <c r="T41" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42">
@@ -4783,7 +4783,7 @@
         <v>15.50387596899225</v>
       </c>
       <c r="T42" t="n">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43">
@@ -4845,7 +4845,7 @@
         <v>7.335907335907336</v>
       </c>
       <c r="T43" t="n">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44">
@@ -4907,7 +4907,7 @@
         <v>18.34862385321101</v>
       </c>
       <c r="T44" t="n">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45">
@@ -4969,7 +4969,7 @@
         <v>2.564102564102564</v>
       </c>
       <c r="T45" t="n">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46">
@@ -5031,7 +5031,7 @@
         <v>12.16931216931217</v>
       </c>
       <c r="T46" t="n">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47">
@@ -5093,7 +5093,7 @@
         <v>25.38461538461538</v>
       </c>
       <c r="T47" t="n">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48">
@@ -5155,7 +5155,7 @@
         <v>31.6</v>
       </c>
       <c r="T48" t="n">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49">
@@ -5217,7 +5217,7 @@
         <v>9.740259740259742</v>
       </c>
       <c r="T49" t="n">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50">
@@ -5279,7 +5279,7 @@
         <v>7.2992700729927</v>
       </c>
       <c r="T50" t="n">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51">
@@ -5341,7 +5341,7 @@
         <v>20.93023255813954</v>
       </c>
       <c r="T51" t="n">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52">
@@ -5403,7 +5403,7 @@
         <v>13.33333333333333</v>
       </c>
       <c r="T52" t="n">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53">
@@ -5465,7 +5465,7 @@
         <v>14.83253588516746</v>
       </c>
       <c r="T53" t="n">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="54">
@@ -5527,7 +5527,7 @@
         <v>12.39669421487603</v>
       </c>
       <c r="T54" t="n">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="55">
@@ -5589,7 +5589,7 @@
         <v>17.3469387755102</v>
       </c>
       <c r="T55" t="n">
-        <v>459</v>
+        <v>447</v>
       </c>
     </row>
     <row r="56">
@@ -5651,7 +5651,7 @@
         <v>10.48158640226629</v>
       </c>
       <c r="T56" t="n">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="57">
@@ -5713,7 +5713,7 @@
         <v>3.141361256544502</v>
       </c>
       <c r="T57" t="n">
-        <v>476</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58">
@@ -5775,7 +5775,7 @@
         <v>15.11627906976744</v>
       </c>
       <c r="T58" t="n">
-        <v>492</v>
+        <v>474</v>
       </c>
     </row>
     <row r="59">
@@ -5837,7 +5837,7 @@
         <v>15.29411764705882</v>
       </c>
       <c r="T59" t="n">
-        <v>510</v>
+        <v>491</v>
       </c>
     </row>
     <row r="60">
@@ -5899,7 +5899,7 @@
         <v>12.92775665399239</v>
       </c>
       <c r="T60" t="n">
-        <v>541</v>
+        <v>522</v>
       </c>
     </row>
     <row r="61">
@@ -5961,7 +5961,7 @@
         <v>9.621993127147768</v>
       </c>
       <c r="T61" t="n">
-        <v>566</v>
+        <v>546</v>
       </c>
     </row>
     <row r="62">
@@ -6023,7 +6023,7 @@
         <v>10.77441077441077</v>
       </c>
       <c r="T62" t="n">
-        <v>597</v>
+        <v>576</v>
       </c>
     </row>
     <row r="63">
@@ -6085,7 +6085,7 @@
         <v>7.555555555555555</v>
       </c>
       <c r="T63" t="n">
-        <v>579</v>
+        <v>557</v>
       </c>
     </row>
     <row r="64">
@@ -6147,7 +6147,7 @@
         <v>4</v>
       </c>
       <c r="T64" t="n">
-        <v>558</v>
+        <v>536</v>
       </c>
     </row>
     <row r="65">
@@ -6209,7 +6209,7 @@
         <v>4</v>
       </c>
       <c r="T65" t="n">
-        <v>550</v>
+        <v>528</v>
       </c>
     </row>
     <row r="66">
@@ -6271,7 +6271,7 @@
         <v>2.892561983471075</v>
       </c>
       <c r="T66" t="n">
-        <v>535</v>
+        <v>513</v>
       </c>
     </row>
     <row r="67">
@@ -6333,7 +6333,7 @@
         <v>3.167420814479638</v>
       </c>
       <c r="T67" t="n">
-        <v>515</v>
+        <v>493</v>
       </c>
     </row>
     <row r="68">
@@ -6395,7 +6395,7 @@
         <v>4.347826086956522</v>
       </c>
       <c r="T68" t="n">
-        <v>487</v>
+        <v>465</v>
       </c>
     </row>
     <row r="69">
@@ -6457,7 +6457,7 @@
         <v>6.796116504854369</v>
       </c>
       <c r="T69" t="n">
-        <v>470</v>
+        <v>445</v>
       </c>
     </row>
     <row r="70">
@@ -6519,7 +6519,7 @@
         <v>1.574803149606299</v>
       </c>
       <c r="T70" t="n">
-        <v>452</v>
+        <v>426</v>
       </c>
     </row>
     <row r="71">
@@ -6581,7 +6581,7 @@
         <v>0.4545454545454545</v>
       </c>
       <c r="T71" t="n">
-        <v>366</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
@@ -6643,7 +6643,7 @@
         <v>1.234567901234568</v>
       </c>
       <c r="T72" t="n">
-        <v>327</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73">
@@ -6705,7 +6705,7 @@
         <v>0.4366812227074235</v>
       </c>
       <c r="T73" t="n">
-        <v>300</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74">
@@ -6767,7 +6767,7 @@
         <v>0.411522633744856</v>
       </c>
       <c r="T74" t="n">
-        <v>240</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75">
@@ -6829,7 +6829,7 @@
         <v>4.519774011299435</v>
       </c>
       <c r="T75" t="n">
-        <v>217</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76">
@@ -6891,7 +6891,7 @@
         <v>7.000000000000001</v>
       </c>
       <c r="T76" t="n">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77">
@@ -6953,7 +6953,7 @@
         <v>5.583756345177665</v>
       </c>
       <c r="T77" t="n">
-        <v>238</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78">
@@ -7015,7 +7015,7 @@
         <v>9.338521400778211</v>
       </c>
       <c r="T78" t="n">
-        <v>248</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79">
@@ -7077,7 +7077,7 @@
         <v>3.137254901960784</v>
       </c>
       <c r="T79" t="n">
-        <v>256</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80">
@@ -7139,7 +7139,7 @@
         <v>6</v>
       </c>
       <c r="T80" t="n">
-        <v>255</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81">
@@ -7201,7 +7201,7 @@
         <v>4.23728813559322</v>
       </c>
       <c r="T81" t="n">
-        <v>264</v>
+        <v>235</v>
       </c>
     </row>
     <row r="82">
@@ -7263,7 +7263,7 @@
         <v>5.651105651105651</v>
       </c>
       <c r="T82" t="n">
-        <v>265</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83">
@@ -7325,7 +7325,7 @@
         <v>3.465346534653466</v>
       </c>
       <c r="T83" t="n">
-        <v>249</v>
+        <v>220</v>
       </c>
     </row>
     <row r="84">
@@ -7387,7 +7387,7 @@
         <v>1.5</v>
       </c>
       <c r="T84" t="n">
-        <v>234</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85">
@@ -7449,7 +7449,7 @@
         <v>0.4739336492890995</v>
       </c>
       <c r="T85" t="n">
-        <v>220</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86">
@@ -7511,7 +7511,7 @@
         <v>6.730769230769231</v>
       </c>
       <c r="T86" t="n">
-        <v>231</v>
+        <v>202</v>
       </c>
     </row>
     <row r="87">
@@ -7573,7 +7573,7 @@
         <v>0.6896551724137931</v>
       </c>
       <c r="T87" t="n">
-        <v>232</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88">
@@ -7635,7 +7635,7 @@
         <v>7.865168539325842</v>
       </c>
       <c r="T88" t="n">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89">
@@ -7697,7 +7697,7 @@
         <v>2.287581699346405</v>
       </c>
       <c r="T89" t="n">
-        <v>247</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90">
@@ -7759,7 +7759,7 @@
         <v>0</v>
       </c>
       <c r="T90" t="n">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="91">
@@ -7821,7 +7821,7 @@
         <v>2.469135802469136</v>
       </c>
       <c r="T91" t="n">
-        <v>247</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92">
@@ -7883,7 +7883,7 @@
         <v>4.090909090909091</v>
       </c>
       <c r="T92" t="n">
-        <v>253</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93">
@@ -7945,7 +7945,7 @@
         <v>0.3745318352059925</v>
       </c>
       <c r="T93" t="n">
-        <v>247</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94">
@@ -8007,7 +8007,7 @@
         <v>1.204819277108434</v>
       </c>
       <c r="T94" t="n">
-        <v>232</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95">
@@ -8069,7 +8069,7 @@
         <v>3.858520900321544</v>
       </c>
       <c r="T95" t="n">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96">
@@ -8131,7 +8131,7 @@
         <v>2.727272727272727</v>
       </c>
       <c r="T96" t="n">
-        <v>229</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97">
@@ -8193,7 +8193,7 @@
         <v>11.50442477876106</v>
       </c>
       <c r="T97" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98">
@@ -8255,7 +8255,7 @@
         <v>15.69767441860465</v>
       </c>
       <c r="T98" t="n">
-        <v>267</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99">
@@ -8317,7 +8317,7 @@
         <v>6.735751295336788</v>
       </c>
       <c r="T99" t="n">
-        <v>276</v>
+        <v>246</v>
       </c>
     </row>
     <row r="100">
@@ -8379,7 +8379,7 @@
         <v>7.5098814229249</v>
       </c>
       <c r="T100" t="n">
-        <v>271</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101">
@@ -8441,7 +8441,7 @@
         <v>1.700680272108844</v>
       </c>
       <c r="T101" t="n">
-        <v>273</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102">
@@ -8503,7 +8503,7 @@
         <v>3.703703703703703</v>
       </c>
       <c r="T102" t="n">
-        <v>282</v>
+        <v>252</v>
       </c>
     </row>
     <row r="103">
@@ -8565,7 +8565,7 @@
         <v>17.91044776119403</v>
       </c>
       <c r="T103" t="n">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="104">
@@ -8627,7 +8627,7 @@
         <v>13.51351351351351</v>
       </c>
       <c r="T104" t="n">
-        <v>344</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105">
@@ -8689,7 +8689,7 @@
         <v>12.55411255411255</v>
       </c>
       <c r="T105" t="n">
-        <v>351</v>
+        <v>320</v>
       </c>
     </row>
     <row r="106">
@@ -8751,7 +8751,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="T106" t="n">
-        <v>357</v>
+        <v>326</v>
       </c>
     </row>
     <row r="107">
@@ -8813,7 +8813,7 @@
         <v>10.35714285714286</v>
       </c>
       <c r="T107" t="n">
-        <v>385</v>
+        <v>354</v>
       </c>
     </row>
     <row r="108">
@@ -8875,7 +8875,7 @@
         <v>12.28070175438596</v>
       </c>
       <c r="T108" t="n">
-        <v>405</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109">
@@ -8937,7 +8937,7 @@
         <v>25.55066079295154</v>
       </c>
       <c r="T109" t="n">
-        <v>463</v>
+        <v>432</v>
       </c>
     </row>
     <row r="110">
@@ -8999,7 +8999,7 @@
         <v>16.93290734824281</v>
       </c>
       <c r="T110" t="n">
-        <v>509</v>
+        <v>477</v>
       </c>
     </row>
     <row r="111">
@@ -9061,7 +9061,7 @@
         <v>18.49056603773585</v>
       </c>
       <c r="T111" t="n">
-        <v>533</v>
+        <v>500</v>
       </c>
     </row>
     <row r="112">
@@ -9123,7 +9123,7 @@
         <v>33.50649350649351</v>
       </c>
       <c r="T112" t="n">
-        <v>652</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>